<commit_message>
Executed the old testcases
</commit_message>
<xml_diff>
--- a/src/test/java/com/impetus/data/RA.xlsx
+++ b/src/test/java/com/impetus/data/RA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinta.anusha/Desktop/UVPAutomation/src/test/java/com/impetus/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117A5C4-2338-BF46-BB16-7AF3B9A8F559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA31214-83E6-E245-9196-3404AF037394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" xr2:uid="{66A29900-7A95-7A43-A1FA-176511A62359}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{66A29900-7A95-7A43-A1FA-176511A62359}"/>
   </bookViews>
   <sheets>
     <sheet name="RAFile" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="27">
   <si>
     <t>Segment</t>
   </si>
@@ -64,30 +64,12 @@
     <t>Enrichment</t>
   </si>
   <si>
-    <t>ASPMin</t>
-  </si>
-  <si>
-    <t>ASPMax</t>
-  </si>
-  <si>
     <t>OptionsCount</t>
   </si>
   <si>
     <t>OTBNumber</t>
   </si>
   <si>
-    <t>ODM Quantity</t>
-  </si>
-  <si>
-    <t>OEM Quantity</t>
-  </si>
-  <si>
-    <t>TotalQty</t>
-  </si>
-  <si>
-    <t>FillPercentage</t>
-  </si>
-  <si>
     <t>Shein Fast Fashion</t>
   </si>
   <si>
@@ -128,6 +110,12 @@
   </si>
   <si>
     <t>MenWesternwearDenimBottomwear</t>
+  </si>
+  <si>
+    <t>MRPMin</t>
+  </si>
+  <si>
+    <t>MRPMax</t>
   </si>
 </sst>
 </file>
@@ -479,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BC677C-F655-D74C-9044-4FF6B3F29943}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,16 +481,13 @@
     <col min="5" max="5" width="19.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="12" max="12" width="39" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,57 +510,45 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
       <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
       </c>
       <c r="H2">
         <v>300</v>
@@ -586,49 +559,37 @@
       <c r="J2">
         <v>30</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2">
         <v>910203002</v>
       </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
       <c r="H3">
         <v>400</v>
@@ -639,49 +600,37 @@
       <c r="J3">
         <v>40</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3">
         <v>910203002</v>
       </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
       </c>
       <c r="H4">
         <v>500</v>
@@ -692,49 +641,37 @@
       <c r="J4">
         <v>30</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4">
         <v>910203002</v>
       </c>
-      <c r="Q4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
       </c>
       <c r="H5">
         <v>600</v>
@@ -745,49 +682,37 @@
       <c r="J5">
         <v>22</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5">
         <v>910203002</v>
       </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
       </c>
       <c r="H6">
         <v>700</v>
@@ -798,49 +723,37 @@
       <c r="J6">
         <v>16</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
       </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6">
         <v>910203002</v>
       </c>
-      <c r="Q6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
       </c>
       <c r="H7">
         <v>800</v>
@@ -851,49 +764,37 @@
       <c r="J7">
         <v>10</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
       </c>
       <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7">
         <v>910203002</v>
       </c>
-      <c r="Q7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
       </c>
       <c r="H8">
         <v>200</v>
@@ -904,49 +805,37 @@
       <c r="J8">
         <v>27</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
       </c>
       <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8">
         <v>910203003</v>
       </c>
-      <c r="Q8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
       </c>
       <c r="H9">
         <v>300</v>
@@ -957,49 +846,37 @@
       <c r="J9">
         <v>40</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
       </c>
       <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9">
         <v>910203003</v>
       </c>
-      <c r="Q9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
       </c>
       <c r="H10">
         <v>400</v>
@@ -1010,49 +887,37 @@
       <c r="J10">
         <v>47</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
       </c>
       <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10">
         <v>910203003</v>
       </c>
-      <c r="Q10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
       </c>
       <c r="H11">
         <v>500</v>
@@ -1063,49 +928,37 @@
       <c r="J11">
         <v>40</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
       </c>
       <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11">
         <v>910203003</v>
       </c>
-      <c r="Q11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H12">
         <v>500</v>
@@ -1116,49 +969,37 @@
       <c r="J12">
         <v>62</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
       </c>
       <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>30</v>
-      </c>
-      <c r="P12">
         <v>910103001</v>
       </c>
-      <c r="Q12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H13">
         <v>600</v>
@@ -1169,49 +1010,37 @@
       <c r="J13">
         <v>187</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
       </c>
       <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13">
         <v>910103001</v>
       </c>
-      <c r="Q13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H14">
         <v>700</v>
@@ -1222,49 +1051,37 @@
       <c r="J14">
         <v>376</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
       </c>
       <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14">
         <v>910103001</v>
       </c>
-      <c r="Q14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H15">
         <v>800</v>
@@ -1275,49 +1092,37 @@
       <c r="J15">
         <v>275</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
       </c>
       <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15">
         <v>910103001</v>
       </c>
-      <c r="Q15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H16">
         <v>900</v>
@@ -1328,49 +1133,37 @@
       <c r="J16">
         <v>226</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
       </c>
       <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>30</v>
-      </c>
-      <c r="P16">
         <v>910103001</v>
       </c>
-      <c r="Q16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <v>1000</v>
@@ -1381,26 +1174,14 @@
       <c r="J17">
         <v>125</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
       </c>
       <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17">
         <v>910103001</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>